<commit_message>
Session 6 files uploaded
</commit_message>
<xml_diff>
--- a/Orientation II.xlsx
+++ b/Orientation II.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA SCIENCE THINKLOGIX ACADEMY\4PM-6PM (SAT) OCT-17-2020 BATCH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA SCIENCE THINKLOGIX ACADEMY\4PM-6PM (SAT) OCT-17-2020 BATCH\Python-II-Oct-17-2020-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{099FD040-44F0-409B-9B24-B0C6B42B1BD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E16874B-60A5-418F-A621-8644792FEE33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OfficeSupplies" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="133">
   <si>
     <t>OrderDate</t>
   </si>
@@ -419,12 +419,15 @@
   </si>
   <si>
     <t>Slow processing in comparison to OLTP</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1027,22 +1030,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1057,9 +1045,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1081,6 +1066,24 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2367,6 +2370,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-8E6B-40C4-87CE-CBFF5C0A2EE4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2382,6 +2390,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-8E6B-40C4-87CE-CBFF5C0A2EE4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2397,6 +2410,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-8E6B-40C4-87CE-CBFF5C0A2EE4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -5168,12 +5186,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5249,21 +5265,21 @@
       <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="26" t="s">
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="14"/>
+      <c r="P3" s="9"/>
       <c r="R3" t="s">
         <v>77</v>
       </c>
@@ -5299,26 +5315,26 @@
       <c r="F4">
         <v>4.99</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16" t="s">
+      <c r="M4" s="11"/>
+      <c r="N4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="17" t="s">
+      <c r="P4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="Q4" s="22" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5341,23 +5357,23 @@
       <c r="F5">
         <v>1.99</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="10">
         <v>1</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16">
+      <c r="M5" s="11"/>
+      <c r="N5" s="11">
         <v>1</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="O5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="17">
+      <c r="P5" s="12">
         <v>2</v>
       </c>
       <c r="Q5" t="s">
@@ -5383,23 +5399,23 @@
       <c r="F6">
         <v>12.49</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="10">
         <v>2</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16">
+      <c r="M6" s="11"/>
+      <c r="N6" s="11">
         <v>2</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="O6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="17">
+      <c r="P6" s="12">
         <v>4</v>
       </c>
       <c r="Q6" t="s">
@@ -5431,23 +5447,23 @@
       <c r="F7">
         <v>19.989999999999998</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="13">
         <v>3</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19">
+      <c r="M7" s="14"/>
+      <c r="N7" s="14">
         <v>3</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="O7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="P7" s="20">
+      <c r="P7" s="15">
         <v>5</v>
       </c>
       <c r="Q7" t="s">
@@ -5479,13 +5495,13 @@
       <c r="F8">
         <v>23.95</v>
       </c>
-      <c r="N8" s="28">
+      <c r="N8" s="22">
         <v>4</v>
       </c>
-      <c r="O8" s="28" t="s">
+      <c r="O8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="35">
+      <c r="P8" s="29">
         <v>2</v>
       </c>
       <c r="Q8" t="s">
@@ -5584,7 +5600,7 @@
       <c r="K11" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="25" t="s">
+      <c r="L11" s="19" t="s">
         <v>36</v>
       </c>
       <c r="M11" t="s">
@@ -5593,20 +5609,20 @@
       <c r="N11" t="s">
         <v>46</v>
       </c>
-      <c r="Q11" s="23" t="s">
+      <c r="Q11" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="R11" s="24" t="s">
+      <c r="R11" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="S11" s="24"/>
-      <c r="U11" s="23" t="s">
+      <c r="S11" s="40"/>
+      <c r="U11" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="V11" s="24" t="s">
+      <c r="V11" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="W11" s="24"/>
+      <c r="W11" s="40"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -5627,7 +5643,7 @@
       <c r="F12">
         <v>1.29</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="16">
         <v>44105</v>
       </c>
       <c r="J12">
@@ -5636,7 +5652,7 @@
       <c r="K12">
         <v>1</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="19">
         <v>3</v>
       </c>
       <c r="M12">
@@ -5686,7 +5702,7 @@
       <c r="F13">
         <v>15.99</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="16">
         <v>44106</v>
       </c>
       <c r="J13">
@@ -5695,7 +5711,7 @@
       <c r="K13">
         <v>3</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="19">
         <v>1</v>
       </c>
       <c r="M13">
@@ -5746,7 +5762,7 @@
       <c r="F14">
         <v>1.99</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="16">
         <v>44106</v>
       </c>
       <c r="J14">
@@ -5755,7 +5771,7 @@
       <c r="K14">
         <v>3</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14" s="19">
         <v>2</v>
       </c>
       <c r="M14">
@@ -5806,7 +5822,7 @@
       <c r="F15">
         <v>8.99</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="16">
         <v>44107</v>
       </c>
       <c r="J15">
@@ -5815,7 +5831,7 @@
       <c r="K15">
         <v>2</v>
       </c>
-      <c r="L15" s="25">
+      <c r="L15" s="19">
         <v>2</v>
       </c>
       <c r="M15">
@@ -5866,11 +5882,11 @@
       <c r="F16">
         <v>19.989999999999998</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="L16" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="M16" s="23"/>
-      <c r="N16" s="22">
+      <c r="M16" s="18"/>
+      <c r="N16" s="17">
         <v>28</v>
       </c>
       <c r="Q16" t="s">
@@ -5954,16 +5970,16 @@
       <c r="F19">
         <v>19.989999999999998</v>
       </c>
-      <c r="J19" s="12" t="s">
+      <c r="J19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="K19" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="14"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="9"/>
       <c r="Q19" t="s">
         <v>62</v>
       </c>
@@ -5999,22 +6015,22 @@
       <c r="F20">
         <v>4.99</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="J20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="16" t="s">
+      <c r="K20" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="L20" s="16" t="s">
+      <c r="L20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="M20" s="16" t="s">
+      <c r="M20" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="N20" s="16" t="s">
+      <c r="N20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="O20" s="17" t="s">
+      <c r="O20" s="12" t="s">
         <v>46</v>
       </c>
       <c r="Q20" t="s">
@@ -6052,22 +6068,22 @@
       <c r="F21">
         <v>4.99</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="10">
         <v>1</v>
       </c>
-      <c r="K21" s="16" t="s">
+      <c r="K21" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="L21" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="16">
+      <c r="M21" s="11">
         <v>2</v>
       </c>
-      <c r="N21" s="16">
+      <c r="N21" s="11">
         <v>5</v>
       </c>
-      <c r="O21" s="17">
+      <c r="O21" s="12">
         <v>10</v>
       </c>
       <c r="Q21" t="s">
@@ -6105,22 +6121,22 @@
       <c r="F22">
         <v>19.989999999999998</v>
       </c>
-      <c r="J22" s="15">
+      <c r="J22" s="10">
         <v>2</v>
       </c>
-      <c r="K22" s="16" t="s">
+      <c r="K22" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="L22" s="16" t="s">
+      <c r="L22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M22" s="16">
+      <c r="M22" s="11">
         <v>3</v>
       </c>
-      <c r="N22" s="16">
+      <c r="N22" s="11">
         <v>2</v>
       </c>
-      <c r="O22" s="17">
+      <c r="O22" s="12">
         <v>6</v>
       </c>
       <c r="U22" t="s">
@@ -6152,32 +6168,32 @@
       <c r="F23">
         <v>1.29</v>
       </c>
-      <c r="J23" s="15">
+      <c r="J23" s="10">
         <v>2</v>
       </c>
-      <c r="K23" s="16" t="s">
+      <c r="K23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="L23" s="16" t="s">
+      <c r="L23" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M23" s="16">
+      <c r="M23" s="11">
         <v>1</v>
       </c>
-      <c r="N23" s="16">
+      <c r="N23" s="11">
         <v>4</v>
       </c>
-      <c r="O23" s="17">
+      <c r="O23" s="12">
         <v>4</v>
       </c>
-      <c r="T23" s="29" t="s">
+      <c r="T23" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="U23" s="30"/>
-      <c r="V23" s="30">
+      <c r="U23" s="24"/>
+      <c r="V23" s="24">
         <v>3</v>
       </c>
-      <c r="W23" s="31">
+      <c r="W23" s="25">
         <v>6</v>
       </c>
     </row>
@@ -6200,32 +6216,32 @@
       <c r="F24">
         <v>4.99</v>
       </c>
-      <c r="J24" s="18">
+      <c r="J24" s="13">
         <v>3</v>
       </c>
-      <c r="K24" s="19" t="s">
+      <c r="K24" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="L24" s="19" t="s">
+      <c r="L24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="M24" s="19">
+      <c r="M24" s="14">
         <v>2</v>
       </c>
-      <c r="N24" s="19">
+      <c r="N24" s="14">
         <v>4</v>
       </c>
-      <c r="O24" s="20">
+      <c r="O24" s="15">
         <v>8</v>
       </c>
-      <c r="T24" s="32" t="s">
+      <c r="T24" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="U24" s="33"/>
-      <c r="V24" s="33">
+      <c r="U24" s="27"/>
+      <c r="V24" s="27">
         <v>5</v>
       </c>
-      <c r="W24" s="34">
+      <c r="W24" s="28">
         <v>22</v>
       </c>
     </row>
@@ -6288,16 +6304,16 @@
       <c r="F27">
         <v>8.99</v>
       </c>
-      <c r="T27" s="36" t="s">
+      <c r="T27" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="U27" s="37" t="s">
+      <c r="U27" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="V27" s="37" t="s">
+      <c r="V27" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="W27" s="38" t="s">
+      <c r="W27" s="32" t="s">
         <v>8</v>
       </c>
     </row>
@@ -6320,16 +6336,16 @@
       <c r="F28">
         <v>19.989999999999998</v>
       </c>
-      <c r="T28" s="39" t="s">
+      <c r="T28" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="U28" s="40" t="s">
+      <c r="U28" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="V28" s="40" t="s">
+      <c r="V28" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="W28" s="41" t="s">
+      <c r="W28" s="35" t="s">
         <v>111</v>
       </c>
     </row>
@@ -6352,16 +6368,16 @@
       <c r="F29">
         <v>15</v>
       </c>
-      <c r="T29" s="42" t="s">
+      <c r="T29" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="U29" s="43" t="s">
+      <c r="U29" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="V29" s="43" t="s">
+      <c r="V29" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="W29" s="44" t="s">
+      <c r="W29" s="38" t="s">
         <v>110</v>
       </c>
     </row>
@@ -6716,7 +6732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6786,10 +6802,10 @@
       <c r="C5" t="s">
         <v>128</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="39" t="s">
         <v>124</v>
       </c>
     </row>
@@ -6811,13 +6827,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="27"/>
+      <c r="C7" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="41"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -6836,7 +6852,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6908,7 +6924,7 @@
       <c r="I3" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="27">
+      <c r="J3" s="21">
         <v>5000</v>
       </c>
       <c r="K3" t="s">
@@ -6937,7 +6953,7 @@
       <c r="I4" t="s">
         <v>96</v>
       </c>
-      <c r="J4" s="27">
+      <c r="J4" s="21">
         <v>100000</v>
       </c>
       <c r="K4" t="s">
@@ -6966,7 +6982,7 @@
       <c r="I5" t="s">
         <v>103</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5" s="21">
         <v>20000</v>
       </c>
       <c r="K5" t="s">
@@ -6992,7 +7008,7 @@
       <c r="I6" t="s">
         <v>102</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="21">
         <v>500</v>
       </c>
       <c r="K6" t="s">
@@ -7201,25 +7217,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -7237,78 +7253,88 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="B9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>